<commit_message>
Delta Wjk is too small in the excel
</commit_message>
<xml_diff>
--- a/NeuralNetwork/ExternalFiles/Nn.xlsx
+++ b/NeuralNetwork/ExternalFiles/Nn.xlsx
@@ -14,8 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +31,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="H69" authorId="0" shapeId="0">
+    <comment ref="H139" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K69" authorId="0" shapeId="0">
+    <comment ref="K139" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>Input</t>
   </si>
@@ -308,12 +307,336 @@
       <t>jk</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <r>
+      <t>H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <t>http://matrixmultiplication.xyz/</t>
+  </si>
+  <si>
+    <r>
+      <t>∂E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>in)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <t>Sigmoid'</t>
+  </si>
+  <si>
+    <r>
+      <t>∂E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔW</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>kl</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∂O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>kl</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∂H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>int</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>H1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∂E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∂E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t xml:space="preserve"> / ∂H2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔW</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Titillium"/>
+      </rPr>
+      <t>jk</t>
+    </r>
+  </si>
+  <si>
+    <t>aici - cand schimbi de mana eroarea se schimba valorile doar pe ultima coloana - ceea ce e gresit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -351,8 +674,20 @@
       <color theme="1"/>
       <name val="Titillium"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Titillium"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Titillium"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +727,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -674,77 +1027,173 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -769,15 +1218,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
+      <xdr:colOff>200024</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>519965</xdr:colOff>
+      <xdr:colOff>510440</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -807,7 +1256,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="819149" y="2019300"/>
+          <a:off x="809624" y="2019300"/>
           <a:ext cx="4234716" cy="1142999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -837,8 +1286,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>31804</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>155629</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -892,13 +1341,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>494264</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -930,6 +1379,67 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="942975" y="6296026"/>
+          <a:ext cx="4085189" cy="2228849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399014</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="https://cdn-images-1.medium.com/max/1600/1*NWb_tAHWvBwJc0hNm0LiUQ.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EA436DA-C610-48C6-BC7B-27EB73C67899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1457325" y="10096500"/>
           <a:ext cx="4085189" cy="2228849"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1295,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:Y168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="T84" sqref="T84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1309,44 +1819,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="13.5" thickBot="1">
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40" t="s">
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40" t="s">
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
     </row>
     <row r="2" spans="1:19" ht="18.75" thickBot="1">
-      <c r="C2" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="39" t="s">
+      <c r="C2" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39" t="s">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="S2" s="43" t="s">
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="S2" s="39" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1402,7 +1912,7 @@
         <f>$I$4*K5+$J$4*K6+$K$4*K7+K8</f>
         <v>2.8230360327250636</v>
       </c>
-      <c r="S3" s="59">
+      <c r="S3" s="53">
         <v>0.01</v>
       </c>
     </row>
@@ -1463,7 +1973,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="59" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1501,7 +2011,7 @@
       <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1">
-      <c r="A6" s="38"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1537,7 +2047,7 @@
       <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A7" s="38"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1655,694 +2165,1759 @@
     </row>
     <row r="12" spans="1:19" s="22" customFormat="1"/>
     <row r="13" spans="1:19" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H13" s="48" t="s">
+      <c r="K13" s="44" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="22" customFormat="1">
-      <c r="H14" s="44">
+      <c r="K14" s="45">
         <f>(-1)*(C11*(1/L4)+(1-C11)*(1/(1-L4)))</f>
         <v>-3.7065529644704216</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" s="22" customFormat="1">
+      <c r="L14" s="46">
+        <v>0</v>
+      </c>
+      <c r="M14" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="22" customFormat="1" ht="15.75">
+      <c r="A15" s="63" t="s">
+        <v>44</v>
+      </c>
       <c r="D15"/>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="62"/>
+      <c r="J15" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="48">
+        <v>0</v>
+      </c>
+      <c r="L15" s="54">
         <v>-0.30099999999999999</v>
       </c>
-      <c r="I15" s="48">
+      <c r="M15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A16" s="64"/>
+      <c r="K16" s="50">
+        <v>0</v>
+      </c>
+      <c r="L16" s="51">
+        <v>0</v>
+      </c>
+      <c r="M16" s="52">
+        <f>(-1)*(E11*(1/N4)+(1-E11)*(1/(1-N4)))</f>
+        <v>-1.6889906479667314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="22" customFormat="1">
+      <c r="L17" s="44">
         <f>(-1)*(D11*(1/M4)+(1-D11)*(1/(1-M4)))</f>
         <v>-1.4755293951978394</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H16" s="46">
+    <row r="18" spans="1:22" s="22" customFormat="1"/>
+    <row r="19" spans="1:22" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="K19" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="22" customFormat="1">
+      <c r="K20" s="45">
+        <f>(EXP(L3)*(EXP(M3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
+        <v>0.15906572440211431</v>
+      </c>
+      <c r="L20" s="46">
+        <v>0</v>
+      </c>
+      <c r="M20" s="47">
+        <v>0</v>
+      </c>
+      <c r="P20" s="56"/>
+    </row>
+    <row r="21" spans="1:22" s="22" customFormat="1" ht="15.75">
+      <c r="A21" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="48">
+        <v>0</v>
+      </c>
+      <c r="L21" s="21">
+        <f>(EXP(M3)*(EXP(L3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
+        <v>0.20392775168086905</v>
+      </c>
+      <c r="M21" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A22" s="64"/>
+      <c r="K22" s="50">
+        <v>0</v>
+      </c>
+      <c r="L22" s="51">
+        <v>0</v>
+      </c>
+      <c r="M22" s="82">
+        <v>0.36849999999999999</v>
+      </c>
+      <c r="N22" s="22">
+        <f>EXP(N3)*(EXP(L3)+EXP(M3))/(EXP(L3)+EXP(M3)+EXP(N3))^2</f>
+        <v>0.24973763855303174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="22" customFormat="1"/>
+    <row r="24" spans="1:22" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:22" s="56" customFormat="1">
+      <c r="G25"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="79">
+        <f>$K14*K$20+$L14*L$21+$M14*M$22</f>
+        <v>-0.58958553232829181</v>
+      </c>
+      <c r="O25" s="84">
+        <f>$K14*K$20+$L14*K$21+$M14*K$22</f>
+        <v>-0.58958553232829181</v>
+      </c>
+      <c r="P25" s="85">
+        <f>$K14*L$20+$L14*L$21+$M14*L$22</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="86">
+        <f>$K14*M$20+$L14*M$21+$M14*M$22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="56" customFormat="1" ht="15.75">
+      <c r="H26" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="62"/>
+      <c r="J26" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="80">
+        <f>$K15*K$20+$L15*L$21+$M15*M$22</f>
+        <v>-6.1382253255941578E-2</v>
+      </c>
+      <c r="O26" s="87">
+        <f>$K15*K$20+$L15*K$21+$M15*K$22</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="88">
+        <f>$K15*L$20+$L15*L$21+$M15*L$22</f>
+        <v>-6.1382253255941578E-2</v>
+      </c>
+      <c r="Q26" s="89">
+        <f>$K15*M$20+$L15*M$21+$M15*M$22</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="S26" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="T26" s="62"/>
+    </row>
+    <row r="27" spans="1:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="81">
+        <f>$K16*K$20+$L16*L$21+$M16*M$22</f>
+        <v>-0.6223930537757405</v>
+      </c>
+      <c r="O27" s="90">
+        <f>$K16*K$20+$L16*K$21+$M16*K$22</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="91">
+        <f>$K16*L$20+$L16*L$21+$M16*L$22</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="83">
+        <f>$K16*M$20+$L16*M$21+$M16*M$22</f>
+        <v>-0.6223930537757405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" s="56" customFormat="1"/>
+    <row r="29" spans="1:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:22" s="56" customFormat="1" ht="16.5" thickBot="1">
+      <c r="G30"/>
+      <c r="H30" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="62"/>
+      <c r="J30" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="67">
+        <f>I4</f>
+        <v>0.9388312894865416</v>
+      </c>
+      <c r="L30" s="68">
+        <f>J4</f>
+        <v>0.94047563402349843</v>
+      </c>
+      <c r="M30" s="69">
+        <f>K4</f>
+        <v>0.9820843048123673</v>
+      </c>
+      <c r="N30" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O30" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="P30" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q30" s="56">
+        <f>I$4</f>
+        <v>0.9388312894865416</v>
+      </c>
+      <c r="R30" s="56">
+        <f>J$4</f>
+        <v>0.94047563402349843</v>
+      </c>
+      <c r="S30" s="56">
+        <f>K$4</f>
+        <v>0.9820843048123673</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" s="56" customFormat="1" ht="15.75">
+      <c r="G31"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="57"/>
+      <c r="Q31" s="56">
+        <f>I$4</f>
+        <v>0.9388312894865416</v>
+      </c>
+      <c r="R31" s="56">
+        <f>J$4</f>
+        <v>0.94047563402349843</v>
+      </c>
+      <c r="S31" s="56">
+        <f>K$4</f>
+        <v>0.9820843048123673</v>
+      </c>
+      <c r="T31" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="V31" s="62"/>
+    </row>
+    <row r="32" spans="1:22" s="56" customFormat="1">
+      <c r="G32"/>
+      <c r="Q32" s="56">
+        <f>I$4</f>
+        <v>0.9388312894865416</v>
+      </c>
+      <c r="R32" s="56">
+        <f>J$4</f>
+        <v>0.94047563402349843</v>
+      </c>
+      <c r="S32" s="56">
+        <f>K$4</f>
+        <v>0.9820843048123673</v>
+      </c>
+    </row>
+    <row r="33" spans="7:21" s="56" customFormat="1">
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="7:21" s="56" customFormat="1">
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="7:21" s="56" customFormat="1">
+      <c r="G36"/>
+      <c r="K36" s="71">
+        <f>$K25*K$30</f>
+        <v>-0.55352134557837929</v>
+      </c>
+      <c r="L36" s="72">
+        <f>$K25*L$30</f>
+        <v>-0.55449082732753208</v>
+      </c>
+      <c r="M36" s="73">
+        <f>$K25*M$30</f>
+        <v>-0.57902269764406</v>
+      </c>
+      <c r="O36" s="71">
+        <f>$O25*Q$30+$P25*Q$31+$Q25*Q$32</f>
+        <v>-0.55352134557837929</v>
+      </c>
+      <c r="P36" s="72">
+        <f>$O25*R$30+$P25*R$31+$Q25*R$32</f>
+        <v>-0.55449082732753208</v>
+      </c>
+      <c r="Q36" s="73">
+        <f>$O25*S$30+$P25*S$31+$Q25*S$32</f>
+        <v>-0.57902269764406</v>
+      </c>
+      <c r="S36" s="92">
+        <f>K36-O36</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="92">
+        <f t="shared" ref="T36:U36" si="0">L36-P36</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="7:21" s="56" customFormat="1" ht="15.75">
+      <c r="G37"/>
+      <c r="H37" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="62"/>
+      <c r="J37" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="58">
+        <f>$K26*K$30</f>
+        <v>-5.7627579975865095E-2</v>
+      </c>
+      <c r="L37" s="57">
+        <f>$K26*L$30</f>
+        <v>-5.7728513548672609E-2</v>
+      </c>
+      <c r="M37" s="74">
+        <f>$K26*M$30</f>
+        <v>-6.0282547516678053E-2</v>
+      </c>
+      <c r="O37" s="58">
+        <f>$O26*Q$30+$P26*Q$31+$Q26*Q$32</f>
+        <v>-5.7627579975865095E-2</v>
+      </c>
+      <c r="P37" s="57">
+        <f>$O26*R$30+$P26*R$31+$Q26*R$32</f>
+        <v>-5.7728513548672609E-2</v>
+      </c>
+      <c r="Q37" s="74">
+        <f>$O26*S$30+$P26*S$31+$Q26*S$32</f>
+        <v>-6.0282547516678053E-2</v>
+      </c>
+      <c r="S37" s="92">
+        <f t="shared" ref="S37:S38" si="1">K37-O37</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="92">
+        <f t="shared" ref="T37:T38" si="2">L37-P37</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="92">
+        <f t="shared" ref="U37:U38" si="3">M37-Q37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G38"/>
+      <c r="K38" s="75">
+        <f>$K27*K$30</f>
+        <v>-0.58432207324374486</v>
+      </c>
+      <c r="L38" s="76">
+        <f>$K27*L$30</f>
+        <v>-0.58534550186156087</v>
+      </c>
+      <c r="M38" s="77">
+        <f>$K27*M$30</f>
+        <v>-0.61124244953739448</v>
+      </c>
+      <c r="O38" s="75">
+        <f>$O27*Q$30+$P27*Q$31+$Q27*Q$32</f>
+        <v>-0.58432207324374486</v>
+      </c>
+      <c r="P38" s="76">
+        <f>$O27*R$30+$P27*R$31+$Q27*R$32</f>
+        <v>-0.58534550186156087</v>
+      </c>
+      <c r="Q38" s="77">
+        <f>$O27*S$30+$P27*S$31+$Q27*S$32</f>
+        <v>-0.61124244953739448</v>
+      </c>
+      <c r="S38" s="92">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="92">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:21" s="56" customFormat="1">
+      <c r="G39"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="57"/>
+    </row>
+    <row r="40" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G40"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="57"/>
+    </row>
+    <row r="41" spans="7:21" s="56" customFormat="1">
+      <c r="G41"/>
+      <c r="K41" s="45">
+        <f>K36*$S$3</f>
+        <v>-5.5352134557837933E-3</v>
+      </c>
+      <c r="L41" s="46">
+        <f>K37*$S$3</f>
+        <v>-5.7627579975865091E-4</v>
+      </c>
+      <c r="M41" s="47">
+        <f>K38*$S$3</f>
+        <v>-5.8432207324374489E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="7:21" s="56" customFormat="1" ht="15.75">
+      <c r="G42"/>
+      <c r="H42" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="60"/>
+      <c r="J42" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" s="48">
+        <f>L36*$S$3</f>
+        <v>-5.5449082732753211E-3</v>
+      </c>
+      <c r="L42" s="21">
+        <f>L37*$S$3</f>
+        <v>-5.7728513548672609E-4</v>
+      </c>
+      <c r="M42" s="49">
+        <f>L38*$S$3</f>
+        <v>-5.8534550186156087E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G43"/>
+      <c r="K43" s="50">
+        <f>M36*$S$3</f>
+        <v>-5.7902269764406001E-3</v>
+      </c>
+      <c r="L43" s="51">
+        <f>M37*$S$3</f>
+        <v>-6.0282547516678057E-4</v>
+      </c>
+      <c r="M43" s="52">
+        <f>M38*$S$3</f>
+        <v>-6.112424495373945E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="7:21" s="56" customFormat="1">
+      <c r="G44"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="55"/>
+    </row>
+    <row r="45" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G45"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="55"/>
+    </row>
+    <row r="46" spans="7:21" s="56" customFormat="1">
+      <c r="G46"/>
+      <c r="K46" s="71">
+        <f>I5-K41</f>
+        <v>0.1055352134557838</v>
+      </c>
+      <c r="L46" s="72">
+        <f t="shared" ref="L46:M46" si="4">J5-L41</f>
+        <v>0.40057627579975869</v>
+      </c>
+      <c r="M46" s="73">
+        <f t="shared" si="4"/>
+        <v>0.80584322073243753</v>
+      </c>
+    </row>
+    <row r="47" spans="7:21" s="56" customFormat="1" ht="15.75">
+      <c r="G47"/>
+      <c r="H47" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="I47" s="78"/>
+      <c r="J47" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K47" s="58">
+        <f>I6-K42</f>
+        <v>0.3055449082732753</v>
+      </c>
+      <c r="L47" s="57">
+        <f>J6-L42</f>
+        <v>0.70057728513548667</v>
+      </c>
+      <c r="M47" s="74">
+        <f>K6-M42</f>
+        <v>0.20585345501861563</v>
+      </c>
+    </row>
+    <row r="48" spans="7:21" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G48"/>
+      <c r="K48" s="75">
+        <f>I7-K43</f>
+        <v>0.5057902269764406</v>
+      </c>
+      <c r="L48" s="76">
+        <f>J7-L43</f>
+        <v>0.20060282547516678</v>
+      </c>
+      <c r="M48" s="77">
+        <f>K7-M43</f>
+        <v>0.90611242449537399</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15" s="56" customFormat="1">
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="7:15" s="56" customFormat="1">
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="7:15" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="7:15" s="56" customFormat="1">
+      <c r="G52"/>
+      <c r="K52" s="71">
+        <f>I5</f>
+        <v>0.1</v>
+      </c>
+      <c r="L52" s="72">
+        <f t="shared" ref="L52:M52" si="5">J5</f>
+        <v>0.4</v>
+      </c>
+      <c r="M52" s="73">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="7:15" s="56" customFormat="1" ht="15.75">
+      <c r="G53"/>
+      <c r="H53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="I53" s="62"/>
+      <c r="J53" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K53" s="58">
+        <f t="shared" ref="K53:K54" si="6">I6</f>
+        <v>0.3</v>
+      </c>
+      <c r="L53" s="57">
+        <f t="shared" ref="L53:L54" si="7">J6</f>
+        <v>0.7</v>
+      </c>
+      <c r="M53" s="74">
+        <f t="shared" ref="M53:M54" si="8">K6</f>
+        <v>0.2</v>
+      </c>
+      <c r="N53" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O53" s="56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="7:15" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G54"/>
+      <c r="K54" s="75">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="76">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="M54" s="77">
+        <f t="shared" si="8"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="7:15" s="56" customFormat="1">
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="7:15" s="56" customFormat="1">
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="7:15" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="7:15" s="56" customFormat="1">
+      <c r="G58"/>
+      <c r="K58" s="71">
+        <f>$O25*K$52+$P25*K$53+$Q25*K$54</f>
+        <v>-5.8958553232829183E-2</v>
+      </c>
+      <c r="L58" s="72">
+        <f t="shared" ref="L58:M58" si="9">$O25*L$52+$P25*L$53+$Q25*L$54</f>
+        <v>-0.23583421293131673</v>
+      </c>
+      <c r="M58" s="73">
+        <f t="shared" si="9"/>
+        <v>-0.47166842586263347</v>
+      </c>
+    </row>
+    <row r="59" spans="7:15" s="56" customFormat="1" ht="15.75">
+      <c r="G59"/>
+      <c r="H59" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="I59" s="62"/>
+      <c r="J59" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K59" s="58">
+        <f t="shared" ref="K59:M59" si="10">$O26*K$52+$P26*K$53+$Q26*K$54</f>
+        <v>-1.8414675976782473E-2</v>
+      </c>
+      <c r="L59" s="57">
+        <f t="shared" si="10"/>
+        <v>-4.2967577279159105E-2</v>
+      </c>
+      <c r="M59" s="74">
+        <f t="shared" si="10"/>
+        <v>-1.2276450651188316E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="7:15" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G60"/>
+      <c r="K60" s="75">
+        <f t="shared" ref="K60:M60" si="11">$O27*K$52+$P27*K$53+$Q27*K$54</f>
+        <v>-0.31119652688787025</v>
+      </c>
+      <c r="L60" s="76">
+        <f t="shared" si="11"/>
+        <v>-0.1244786107551481</v>
+      </c>
+      <c r="M60" s="77">
+        <f t="shared" si="11"/>
+        <v>-0.56015374839816645</v>
+      </c>
+    </row>
+    <row r="61" spans="7:15" s="56" customFormat="1">
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="7:15" s="56" customFormat="1">
+      <c r="G62"/>
+    </row>
+    <row r="63" spans="7:15" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G63"/>
+      <c r="K63" s="56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="7:15" s="56" customFormat="1">
+      <c r="G64"/>
+      <c r="K64" s="71">
+        <f>1/(1+EXP(I3))*(1-1/(1+EXP(I3)))</f>
+        <v>5.7427099367579122E-2</v>
+      </c>
+      <c r="L64" s="72">
+        <v>0</v>
+      </c>
+      <c r="M64" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="7:22" s="56" customFormat="1" ht="15.75">
+      <c r="G65"/>
+      <c r="H65" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="62"/>
+      <c r="J65" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K65" s="58">
+        <v>0</v>
+      </c>
+      <c r="L65" s="57">
+        <f>1/(1+EXP(J3))*(1-1/(1+EXP(J3)))</f>
+        <v>5.5981215831597007E-2</v>
+      </c>
+      <c r="M65" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G66"/>
+      <c r="K66" s="75">
+        <v>0</v>
+      </c>
+      <c r="L66" s="76">
+        <v>0</v>
+      </c>
+      <c r="M66" s="77">
+        <f>1/(1+EXP(K3))*(1-1/(1+EXP(K3)))</f>
+        <v>1.7594723053576653E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="7:22" s="56" customFormat="1">
+      <c r="G67"/>
+    </row>
+    <row r="68" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G68"/>
+    </row>
+    <row r="69" spans="7:22" s="56" customFormat="1">
+      <c r="G69"/>
+      <c r="K69" s="71">
+        <f>$K58*K$64+$L58*K$65+$M58*K$66</f>
+        <v>-3.385818695070385E-3</v>
+      </c>
+      <c r="L69" s="72">
+        <f t="shared" ref="L69:M69" si="12">$K58*L$64+$L58*L$65+$M58*L$66</f>
+        <v>-1.3202285974582848E-2</v>
+      </c>
+      <c r="M69" s="73">
+        <f t="shared" si="12"/>
+        <v>-8.2988753261694879E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="7:22" s="56" customFormat="1" ht="15.75">
+      <c r="G70"/>
+      <c r="H70" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I70" s="62"/>
+      <c r="J70" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" s="58">
+        <f t="shared" ref="K70:M70" si="13">$K59*K$64+$L59*K$65+$M59*K$66</f>
+        <v>-1.0575014271404593E-3</v>
+      </c>
+      <c r="L70" s="57">
+        <f t="shared" si="13"/>
+        <v>-2.4053772174254294E-3</v>
+      </c>
+      <c r="M70" s="74">
+        <f t="shared" si="13"/>
+        <v>-2.160007492885592E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G71"/>
+      <c r="K71" s="75">
+        <f t="shared" ref="K71:M71" si="14">$K60*K$64+$L60*K$65+$M60*K$66</f>
+        <v>-1.7871113872435233E-2</v>
+      </c>
+      <c r="L71" s="76">
+        <f t="shared" si="14"/>
+        <v>-6.9684639751012986E-3</v>
+      </c>
+      <c r="M71" s="77">
+        <f t="shared" si="14"/>
+        <v>-9.8557500704885958E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="7:22" s="56" customFormat="1">
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="7:22" s="56" customFormat="1" ht="16.5" thickBot="1">
+      <c r="G74"/>
+      <c r="H74" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" s="62"/>
+      <c r="J74" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K74" s="67">
+        <f>F4</f>
+        <v>1.35</v>
+      </c>
+      <c r="L74" s="68">
+        <f t="shared" ref="L74:M74" si="15">G4</f>
+        <v>1.27</v>
+      </c>
+      <c r="M74" s="69">
+        <f t="shared" si="15"/>
+        <v>1.8</v>
+      </c>
+      <c r="N74" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O74" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q74" s="71">
+        <f>F4</f>
+        <v>1.35</v>
+      </c>
+      <c r="R74" s="72">
+        <f t="shared" ref="R74:S74" si="16">G4</f>
+        <v>1.27</v>
+      </c>
+      <c r="S74" s="73">
+        <f t="shared" si="16"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="75" spans="7:22" s="56" customFormat="1" ht="15.75">
+      <c r="G75"/>
+      <c r="Q75" s="58">
+        <f>Q74</f>
+        <v>1.35</v>
+      </c>
+      <c r="R75" s="57">
+        <f t="shared" ref="R75:S75" si="17">R74</f>
+        <v>1.27</v>
+      </c>
+      <c r="S75" s="74">
+        <f t="shared" si="17"/>
+        <v>1.8</v>
+      </c>
+      <c r="T75" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="U75" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="V75" s="62"/>
+    </row>
+    <row r="76" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G76"/>
+      <c r="Q76" s="75">
+        <f>Q75</f>
+        <v>1.35</v>
+      </c>
+      <c r="R76" s="76">
+        <f t="shared" ref="R76" si="18">R75</f>
+        <v>1.27</v>
+      </c>
+      <c r="S76" s="77">
+        <f t="shared" ref="S76" si="19">S75</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="77" spans="7:22" s="56" customFormat="1">
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="7:22" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="7:22" s="56" customFormat="1">
+      <c r="G79"/>
+      <c r="K79" s="71">
+        <f>$K69*Q$74+$L69*Q$75+$M69*Q$76</f>
+        <v>-3.3597422994360679E-2</v>
+      </c>
+      <c r="L79" s="72">
+        <f t="shared" ref="L79:M79" si="20">$K69*R$74+$L69*R$75+$M69*R$76</f>
+        <v>-3.1606464594694857E-2</v>
+      </c>
+      <c r="M79" s="73">
+        <f t="shared" si="20"/>
+        <v>-4.4796563992480901E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="7:22" s="56" customFormat="1" ht="15.75">
+      <c r="G80"/>
+      <c r="H80" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="I80" s="62"/>
+      <c r="J80" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K80" s="58">
+        <f t="shared" ref="K80:K81" si="21">$K70*Q$74+$L70*Q$75+$M70*Q$76</f>
+        <v>-4.966487181703505E-3</v>
+      </c>
+      <c r="L80" s="57">
+        <f t="shared" ref="L80:L81" si="22">$K70*R$74+$L70*R$75+$M70*R$76</f>
+        <v>-4.6721768301951488E-3</v>
+      </c>
+      <c r="M80" s="74">
+        <f t="shared" ref="M80:M81" si="23">$K70*S$74+$L70*S$75+$M70*S$76</f>
+        <v>-6.6219829089380067E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:25" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G81"/>
+      <c r="K81" s="75">
+        <f t="shared" si="21"/>
+        <v>-4.6838692689333931E-2</v>
+      </c>
+      <c r="L81" s="76">
+        <f t="shared" si="22"/>
+        <v>-4.4063066455891912E-2</v>
+      </c>
+      <c r="M81" s="77">
+        <f t="shared" si="23"/>
+        <v>-6.2451590252445233E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:25" s="56" customFormat="1">
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="2:25" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="2:25" s="56" customFormat="1">
+      <c r="G84"/>
+      <c r="K84" s="45">
+        <f>K79*$S$3</f>
+        <v>-3.359742299436068E-4</v>
+      </c>
+      <c r="L84" s="46">
+        <f>K80*$S$3</f>
+        <v>-4.9664871817035052E-5</v>
+      </c>
+      <c r="M84" s="47">
+        <f>K81*$S$3</f>
+        <v>-4.6838692689333931E-4</v>
+      </c>
+      <c r="O84" s="55">
+        <v>-3.359742299436068E-4</v>
+      </c>
+      <c r="P84" s="55">
+        <v>-4.9664871817035052E-5</v>
+      </c>
+      <c r="Q84" s="55">
+        <v>-4.6838692689333931E-4</v>
+      </c>
+      <c r="S84" s="56">
+        <f>K84-O84</f>
+        <v>0</v>
+      </c>
+      <c r="T84" s="56">
+        <f t="shared" ref="T84:U84" si="24">L84-P84</f>
+        <v>0</v>
+      </c>
+      <c r="U84" s="56">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:25" s="56" customFormat="1" ht="15.75">
+      <c r="G85"/>
+      <c r="H85" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="I85" s="60"/>
+      <c r="J85" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K85" s="48">
+        <f>L79*$S$3</f>
+        <v>-3.1606464594694856E-4</v>
+      </c>
+      <c r="L85" s="21">
+        <f>L80*$S$3</f>
+        <v>-4.6721768301951487E-5</v>
+      </c>
+      <c r="M85" s="49">
+        <f>L81*$S$3</f>
+        <v>-4.4063066455891914E-4</v>
+      </c>
+      <c r="O85" s="55">
+        <v>-3.1606464594694856E-4</v>
+      </c>
+      <c r="P85" s="55">
+        <v>-4.6721768301951487E-5</v>
+      </c>
+      <c r="Q85" s="55">
+        <v>-4.4063066455891914E-4</v>
+      </c>
+      <c r="S85" s="56">
+        <f t="shared" ref="S85:S86" si="25">K85-O85</f>
+        <v>0</v>
+      </c>
+      <c r="T85" s="56">
+        <f t="shared" ref="T85:T86" si="26">L85-P85</f>
+        <v>0</v>
+      </c>
+      <c r="U85" s="56">
+        <f t="shared" ref="U85:U86" si="27">M85-Q85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:25" s="56" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G86"/>
+      <c r="K86" s="50">
+        <f>M79*$S$3</f>
+        <v>-4.4796563992480904E-4</v>
+      </c>
+      <c r="L86" s="51">
+        <f>M80*$S$3</f>
+        <v>-6.6219829089380074E-5</v>
+      </c>
+      <c r="M86" s="52">
+        <f>M81*$S$3</f>
+        <v>-6.2451590252445238E-4</v>
+      </c>
+      <c r="O86" s="55">
+        <v>-4.4796563992480904E-4</v>
+      </c>
+      <c r="P86" s="55">
+        <v>-6.6219829089380074E-5</v>
+      </c>
+      <c r="Q86" s="55">
+        <v>-6.2451590252445238E-4</v>
+      </c>
+      <c r="S86" s="56">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="T86" s="56">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="U86" s="56">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:25" s="56" customFormat="1">
+      <c r="G87"/>
+      <c r="K87" s="93" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="2:25" s="56" customFormat="1">
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="2:25" s="56" customFormat="1">
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="2:25" s="56" customFormat="1">
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="2:25" s="56" customFormat="1">
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="2:25" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="2:25" s="22" customFormat="1">
+      <c r="G93"/>
+      <c r="H93" s="45">
+        <f>$K20*I$4</f>
+        <v>0.14933587915354782</v>
+      </c>
+      <c r="I93" s="46">
+        <f>$K20*J$4</f>
+        <v>0.14959743800848552</v>
+      </c>
+      <c r="J93" s="47">
+        <f>$K20*K$4</f>
+        <v>0.15621595136892605</v>
+      </c>
+      <c r="X93" s="56"/>
+      <c r="Y93" s="56"/>
+    </row>
+    <row r="94" spans="2:25" s="22" customFormat="1" ht="15.75">
+      <c r="B94" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E94" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="F94" s="62"/>
+      <c r="G94" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H94" s="48">
+        <f>$L21*I$4</f>
+        <v>0.19145375407264154</v>
+      </c>
+      <c r="I94" s="21">
+        <f>$L21*J$4</f>
+        <v>0.19178908155705188</v>
+      </c>
+      <c r="J94" s="49">
+        <f>$L21*K$4</f>
+        <v>0.20027424424145535</v>
+      </c>
+      <c r="K94" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="L94" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="M94" s="66"/>
+      <c r="S94" s="43"/>
+      <c r="W94" s="56"/>
+      <c r="X94" s="56"/>
+      <c r="Y94" s="56"/>
+    </row>
+    <row r="95" spans="2:25" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G95"/>
+      <c r="H95" s="50">
+        <f>$M22*I$4</f>
+        <v>0.34595933017579056</v>
+      </c>
+      <c r="I95" s="51">
+        <f>$M22*J$4</f>
+        <v>0.34656527113765917</v>
+      </c>
+      <c r="J95" s="52">
+        <f>$M22*K$4</f>
+        <v>0.36189806632335736</v>
+      </c>
+      <c r="W95" s="56"/>
+      <c r="X95" s="56"/>
+      <c r="Y95" s="56"/>
+    </row>
+    <row r="96" spans="2:25" s="56" customFormat="1">
+      <c r="G96"/>
+      <c r="I96" s="55"/>
+      <c r="J96" s="55"/>
+    </row>
+    <row r="97" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="5:15" s="22" customFormat="1">
+      <c r="G98"/>
+      <c r="H98" s="45">
+        <f>$K14*H$93+$L14*H$94+$M14*H$95</f>
+        <v>-0.55352134557837929</v>
+      </c>
+      <c r="I98" s="46">
+        <f>$K14*I$93+$L14*I$94+$M14*I$95</f>
+        <v>-0.55449082732753208</v>
+      </c>
+      <c r="J98" s="47">
+        <f>$K14*J$93+$L14*J$94+$M14*J$95</f>
+        <v>-0.57902269764406011</v>
+      </c>
+      <c r="M98" s="45">
+        <f>H98</f>
+        <v>-0.55352134557837929</v>
+      </c>
+      <c r="N98" s="46">
+        <f>H99</f>
+        <v>-5.7627579975865102E-2</v>
+      </c>
+      <c r="O98" s="47">
+        <f>H100</f>
+        <v>-0.58432207324374486</v>
+      </c>
+    </row>
+    <row r="99" spans="5:15" s="22" customFormat="1" ht="15.75">
+      <c r="E99" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="62"/>
+      <c r="G99" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H99" s="48">
+        <f>$K15*H$93+$L15*H$94+$M15*H$95</f>
+        <v>-5.7627579975865102E-2</v>
+      </c>
+      <c r="I99" s="21">
+        <f>$K15*I$93+$L15*I$94+$M15*I$95</f>
+        <v>-5.7728513548672616E-2</v>
+      </c>
+      <c r="J99" s="49">
+        <f>$K15*J$93+$L15*J$94+$M15*J$95</f>
+        <v>-6.028254751667806E-2</v>
+      </c>
+      <c r="K99" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="L99" s="60"/>
+      <c r="M99" s="48">
+        <f>I98</f>
+        <v>-0.55449082732753208</v>
+      </c>
+      <c r="N99" s="21">
+        <f>I99</f>
+        <v>-5.7728513548672616E-2</v>
+      </c>
+      <c r="O99" s="49">
+        <f>I100</f>
+        <v>-0.58534550186156087</v>
+      </c>
+    </row>
+    <row r="100" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H100" s="50">
+        <f>$K16*H$93+$L16*H$94+$M16*H$95</f>
+        <v>-0.58432207324374486</v>
+      </c>
+      <c r="I100" s="51">
+        <f>$K16*I$93+$L16*I$94+$M16*I$95</f>
+        <v>-0.58534550186156087</v>
+      </c>
+      <c r="J100" s="52">
+        <f>$K16*J$93+$L16*J$94+$M16*J$95</f>
+        <v>-0.61124244953739448</v>
+      </c>
+      <c r="M100" s="50">
+        <f>J98</f>
+        <v>-0.57902269764406011</v>
+      </c>
+      <c r="N100" s="51">
+        <f>J99</f>
+        <v>-6.028254751667806E-2</v>
+      </c>
+      <c r="O100" s="52">
+        <f>J100</f>
+        <v>-0.61124244953739448</v>
+      </c>
+    </row>
+    <row r="101" spans="5:15" s="22" customFormat="1"/>
+    <row r="102" spans="5:15" s="56" customFormat="1" ht="13.5" thickBot="1"/>
+    <row r="103" spans="5:15" s="22" customFormat="1">
+      <c r="H103" s="45">
+        <f>I5-($S$3*M98)</f>
+        <v>0.1055352134557838</v>
+      </c>
+      <c r="I103" s="46">
+        <f>J5-($S$3*N98)</f>
+        <v>0.40057627579975869</v>
+      </c>
+      <c r="J103" s="47">
+        <f>K5-($S$3*O98)</f>
+        <v>0.80584322073243753</v>
+      </c>
+    </row>
+    <row r="104" spans="5:15" s="22" customFormat="1" ht="15.75">
+      <c r="E104" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="62"/>
+      <c r="G104" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H104" s="48">
+        <f>I6-($S$3*M99)</f>
+        <v>0.3055449082732753</v>
+      </c>
+      <c r="I104" s="21">
+        <f>J6-($S$3*N99)</f>
+        <v>0.70057728513548667</v>
+      </c>
+      <c r="J104" s="49">
+        <f>K6-($S$3*O99)</f>
+        <v>0.20585345501861563</v>
+      </c>
+    </row>
+    <row r="105" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H105" s="50">
+        <f>I7-($S$3*M100)</f>
+        <v>0.5057902269764406</v>
+      </c>
+      <c r="I105" s="51">
+        <f>J7-($S$3*N100)</f>
+        <v>0.20060282547516678</v>
+      </c>
+      <c r="J105" s="52">
+        <f>K7-($S$3*O100)</f>
+        <v>0.90611242449537399</v>
+      </c>
+    </row>
+    <row r="106" spans="5:15" s="22" customFormat="1"/>
+    <row r="107" spans="5:15" s="22" customFormat="1"/>
+    <row r="108" spans="5:15" s="22" customFormat="1">
+      <c r="E108"/>
+    </row>
+    <row r="109" spans="5:15" s="22" customFormat="1"/>
+    <row r="110" spans="5:15" s="22" customFormat="1"/>
+    <row r="111" spans="5:15" s="22" customFormat="1"/>
+    <row r="112" spans="5:15" s="22" customFormat="1"/>
+    <row r="113" spans="5:10" s="22" customFormat="1"/>
+    <row r="114" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H114" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="5:10" s="22" customFormat="1">
+      <c r="H115" s="40">
+        <f>1/(1+EXP(I3))*(1-1/(1+EXP(I3)))</f>
+        <v>5.7427099367579122E-2</v>
+      </c>
+      <c r="J115" s="56"/>
+    </row>
+    <row r="116" spans="5:10" s="22" customFormat="1">
+      <c r="G116" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H116" s="41">
+        <f>1/(1+EXP(J3))*(1-1/(1+EXP(J3)))</f>
+        <v>5.5981215831597007E-2</v>
+      </c>
+      <c r="J116" s="56"/>
+    </row>
+    <row r="117" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H117" s="42">
+        <f>1/(1+EXP(K3))*(1-1/(1+EXP(K3)))</f>
+        <v>1.7594723053576653E-2</v>
+      </c>
+      <c r="J117" s="56"/>
+    </row>
+    <row r="118" spans="5:10" s="22" customFormat="1"/>
+    <row r="119" spans="5:10" s="22" customFormat="1"/>
+    <row r="120" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
+    <row r="121" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1">
+      <c r="G121"/>
+      <c r="H121" s="45">
+        <f>$K20*F$4</f>
+        <v>0.21473872794285434</v>
+      </c>
+      <c r="I121" s="46">
+        <f>$K20*G$4</f>
+        <v>0.20201346999068517</v>
+      </c>
+      <c r="J121" s="47">
+        <f>$K20*H$4</f>
+        <v>0.28631830392380575</v>
+      </c>
+    </row>
+    <row r="122" spans="5:10" s="22" customFormat="1" ht="15.75">
+      <c r="E122" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="F122" s="62"/>
+      <c r="G122" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H122" s="48">
+        <f>$L21*F$4</f>
+        <v>0.27530246476917325</v>
+      </c>
+      <c r="I122" s="21">
+        <f>$L21*G$4</f>
+        <v>0.25898824463470371</v>
+      </c>
+      <c r="J122" s="49">
+        <f>$L21*H$4</f>
+        <v>0.36706995302556428</v>
+      </c>
+    </row>
+    <row r="123" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1" thickBot="1">
+      <c r="G123"/>
+      <c r="H123" s="50">
+        <f>$M22*F$4</f>
+        <v>0.497475</v>
+      </c>
+      <c r="I123" s="51">
+        <f>$M22*G$4</f>
+        <v>0.46799499999999999</v>
+      </c>
+      <c r="J123" s="52">
+        <f>$M22*H$4</f>
+        <v>0.6633</v>
+      </c>
+    </row>
+    <row r="124" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1"/>
+    <row r="125" spans="5:10" s="56" customFormat="1" ht="12" customHeight="1"/>
+    <row r="126" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1"/>
+    <row r="127" spans="5:10" s="22" customFormat="1" ht="15.75">
+      <c r="E127" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F127" s="62"/>
+      <c r="G127" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="128" spans="5:10" s="22" customFormat="1" ht="12" customHeight="1"/>
+    <row r="129" spans="1:14" s="22" customFormat="1" ht="12" customHeight="1"/>
+    <row r="130" spans="1:14" s="22" customFormat="1" ht="12" customHeight="1"/>
+    <row r="131" spans="1:14" s="22" customFormat="1"/>
+    <row r="132" spans="1:14" s="22" customFormat="1"/>
+    <row r="133" spans="1:14" s="22" customFormat="1">
+      <c r="N133" s="38">
+        <f>EXP(N3)*(EXP(L3)+EXP(M3))/(EXP(L3)+EXP(M3)+EXP(N3))^2</f>
+        <v>0.24973763855303174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" s="2" customFormat="1">
+      <c r="B134" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I134" s="2">
+        <f>1/(1+EXP(I3))*(1-1/(1+EXP(I3)))</f>
+        <v>5.7427099367579122E-2</v>
+      </c>
+      <c r="J134" s="2">
+        <f>1/(1+EXP(J3))*(1-1/(1+EXP(J3)))</f>
+        <v>5.5981215831597007E-2</v>
+      </c>
+      <c r="K134" s="2">
+        <f>1/(1+EXP(K3))*(1-1/(1+EXP(K3)))</f>
+        <v>1.7594723053576653E-2</v>
+      </c>
+      <c r="L134" s="2">
+        <f>(EXP(L3)*(EXP(M3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
+        <v>0.15906572440211431</v>
+      </c>
+      <c r="M134" s="2">
+        <f>(EXP(M3)*(EXP(L3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
+        <v>0.20392775168086905</v>
+      </c>
+      <c r="N134" s="24">
+        <v>0.36849999999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" s="35" customFormat="1">
+      <c r="A135" s="37"/>
+      <c r="B135" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L135" s="35">
+        <f>SUM(L136:L138)</f>
+        <v>-3.7065529644704216</v>
+      </c>
+      <c r="M135" s="35">
+        <f>SUM(M136:M138)</f>
+        <v>-1.4755293951978394</v>
+      </c>
+      <c r="N135" s="35">
+        <f>SUM(N136:N138)</f>
+        <v>-1.6889906479667314</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" s="3" customFormat="1">
+      <c r="A136" s="36"/>
+      <c r="B136" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I136" s="3">
+        <f>L136*L134*I139</f>
+        <v>-0.55352134557837929</v>
+      </c>
+      <c r="L136" s="3">
+        <f>(-1)*(C11*(1/L4)+(1-C11)*(1/(1-L4)))</f>
+        <v>-3.7065529644704216</v>
+      </c>
+      <c r="M136" s="3">
+        <v>0</v>
+      </c>
+      <c r="N136" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" s="3" customFormat="1">
+      <c r="A137" s="36"/>
+      <c r="B137" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L137" s="3">
+        <v>0</v>
+      </c>
+      <c r="M137" s="3">
+        <f>(-1)*(D11*(1/M4)+(1-D11)*(1/(1-M4)))</f>
+        <v>-1.4755293951978394</v>
+      </c>
+      <c r="N137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A138" s="36"/>
+      <c r="B138" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L138" s="3">
+        <v>0</v>
+      </c>
+      <c r="M138" s="3">
+        <v>0</v>
+      </c>
+      <c r="N138" s="3">
         <f>(-1)*(E11*(1/N4)+(1-E11)*(1/(1-N4)))</f>
         <v>-1.6889906479667314</v>
       </c>
     </row>
-    <row r="17" spans="5:15" s="22" customFormat="1"/>
-    <row r="18" spans="5:15" s="22" customFormat="1"/>
-    <row r="19" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H19" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15" s="22" customFormat="1">
-      <c r="H20" s="44">
-        <f>(EXP(L3)*(EXP(M3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
-        <v>0.15906572440211431</v>
-      </c>
-    </row>
-    <row r="21" spans="5:15" s="22" customFormat="1">
-      <c r="G21" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="45">
-        <f>(EXP(M3)*(EXP(L3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
-        <v>0.20392775168086905</v>
-      </c>
-    </row>
-    <row r="22" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H22" s="49">
-        <v>0.36849999999999999</v>
-      </c>
-      <c r="I22" s="22">
-        <f>EXP(N3)*(EXP(L3)+EXP(M3))/(EXP(L3)+EXP(M3)+EXP(N3))^2</f>
-        <v>0.24973763855303174</v>
-      </c>
-    </row>
-    <row r="23" spans="5:15" s="22" customFormat="1"/>
-    <row r="24" spans="5:15" s="22" customFormat="1">
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="5:15" s="22" customFormat="1">
-      <c r="G26"/>
-      <c r="H26" s="51">
-        <f>I4</f>
-        <v>0.9388312894865416</v>
-      </c>
-      <c r="I26" s="52">
-        <f t="shared" ref="I26:J26" si="0">J4</f>
-        <v>0.94047563402349843</v>
-      </c>
-      <c r="J26" s="53">
-        <f t="shared" si="0"/>
-        <v>0.9820843048123673</v>
-      </c>
-    </row>
-    <row r="27" spans="5:15" s="22" customFormat="1" ht="15.75">
-      <c r="E27" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="50"/>
-      <c r="G27" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="54">
-        <f>H26</f>
-        <v>0.9388312894865416</v>
-      </c>
-      <c r="I27" s="21">
-        <f t="shared" ref="I27:J27" si="1">I26</f>
-        <v>0.94047563402349843</v>
-      </c>
-      <c r="J27" s="55">
-        <f t="shared" si="1"/>
-        <v>0.9820843048123673</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="G28"/>
-      <c r="H28" s="56">
-        <f>H27</f>
-        <v>0.9388312894865416</v>
-      </c>
-      <c r="I28" s="57">
-        <f t="shared" ref="I28" si="2">I27</f>
-        <v>0.94047563402349843</v>
-      </c>
-      <c r="J28" s="58">
-        <f t="shared" ref="J28" si="3">J27</f>
-        <v>0.9820843048123673</v>
-      </c>
-    </row>
-    <row r="29" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="5:15" s="22" customFormat="1">
-      <c r="G30"/>
-      <c r="H30" s="51">
-        <f>H26*$H20*$H14</f>
-        <v>-0.55352134557837929</v>
-      </c>
-      <c r="I30" s="52">
-        <f t="shared" ref="I30:J32" si="4">I26*$H20*$H14</f>
-        <v>-0.55449082732753208</v>
-      </c>
-      <c r="J30" s="53">
-        <f t="shared" si="4"/>
-        <v>-0.57902269764406011</v>
-      </c>
-      <c r="M30" s="51">
-        <f>H30</f>
-        <v>-0.55352134557837929</v>
-      </c>
-      <c r="N30" s="52">
-        <f>H31</f>
-        <v>-5.7627579975865102E-2</v>
-      </c>
-      <c r="O30" s="53">
-        <f>H32</f>
-        <v>-0.58432207324374486</v>
-      </c>
-    </row>
-    <row r="31" spans="5:15" s="22" customFormat="1" ht="15.75">
-      <c r="E31" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="50"/>
-      <c r="G31" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="54">
-        <f>H27*$H21*$H15</f>
-        <v>-5.7627579975865102E-2</v>
-      </c>
-      <c r="I31" s="21">
-        <f t="shared" si="4"/>
-        <v>-5.7728513548672616E-2</v>
-      </c>
-      <c r="J31" s="55">
-        <f t="shared" si="4"/>
-        <v>-6.028254751667806E-2</v>
-      </c>
-      <c r="K31" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="54">
-        <f>I30</f>
-        <v>-0.55449082732753208</v>
-      </c>
-      <c r="N31" s="21">
-        <f>I31</f>
-        <v>-5.7728513548672616E-2</v>
-      </c>
-      <c r="O31" s="55">
-        <f>I32</f>
-        <v>-0.58534550186156087</v>
-      </c>
-    </row>
-    <row r="32" spans="5:15" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H32" s="56">
-        <f>H28*$H22*$H16</f>
-        <v>-0.58432207324374486</v>
-      </c>
-      <c r="I32" s="57">
-        <f t="shared" si="4"/>
-        <v>-0.58534550186156087</v>
-      </c>
-      <c r="J32" s="58">
-        <f t="shared" si="4"/>
-        <v>-0.61124244953739448</v>
-      </c>
-      <c r="M32" s="56">
-        <f>J30</f>
-        <v>-0.57902269764406011</v>
-      </c>
-      <c r="N32" s="57">
-        <f>J31</f>
-        <v>-6.028254751667806E-2</v>
-      </c>
-      <c r="O32" s="58">
-        <f>J32</f>
-        <v>-0.61124244953739448</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="34" spans="5:10" s="22" customFormat="1">
-      <c r="H34" s="51">
-        <f>I5-($S$3*M30)</f>
-        <v>0.1055352134557838</v>
-      </c>
-      <c r="I34" s="52">
-        <f t="shared" ref="I34:J34" si="5">J5-($S$3*N30)</f>
-        <v>0.40057627579975869</v>
-      </c>
-      <c r="J34" s="53">
-        <f t="shared" si="5"/>
-        <v>0.80584322073243753</v>
-      </c>
-    </row>
-    <row r="35" spans="5:10" s="22" customFormat="1" ht="15.75">
-      <c r="E35" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H35" s="54">
-        <f t="shared" ref="H35:H36" si="6">I6-($S$3*M31)</f>
-        <v>0.3055449082732753</v>
-      </c>
-      <c r="I35" s="21">
-        <f t="shared" ref="I35:I36" si="7">J6-($S$3*N31)</f>
-        <v>0.70057728513548667</v>
-      </c>
-      <c r="J35" s="55">
-        <f t="shared" ref="J35:J36" si="8">K6-($S$3*O31)</f>
-        <v>0.20585345501861563</v>
-      </c>
-    </row>
-    <row r="36" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H36" s="56">
-        <f t="shared" si="6"/>
-        <v>0.5057902269764406</v>
-      </c>
-      <c r="I36" s="57">
-        <f t="shared" si="7"/>
-        <v>0.20060282547516678</v>
-      </c>
-      <c r="J36" s="58">
-        <f t="shared" si="8"/>
-        <v>0.90611242449537399</v>
-      </c>
-    </row>
-    <row r="37" spans="5:10" s="22" customFormat="1"/>
-    <row r="38" spans="5:10" s="22" customFormat="1"/>
-    <row r="39" spans="5:10" s="22" customFormat="1">
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="5:10" s="22" customFormat="1"/>
-    <row r="41" spans="5:10" s="22" customFormat="1"/>
-    <row r="42" spans="5:10" s="22" customFormat="1"/>
-    <row r="43" spans="5:10" s="22" customFormat="1"/>
-    <row r="44" spans="5:10" s="22" customFormat="1"/>
-    <row r="45" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="46" spans="5:10" s="22" customFormat="1">
-      <c r="H46" s="44">
-        <f>1/(1+EXP(I3))*(1-1/(1+EXP(I3)))</f>
-        <v>5.7427099367579122E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="5:10" s="22" customFormat="1">
-      <c r="G47" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H47" s="45">
-        <f>1/(1+EXP(J3))*(1-1/(1+EXP(J3)))</f>
-        <v>5.5981215831597007E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="5:10" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H48" s="46">
-        <f>1/(1+EXP(K3))*(1-1/(1+EXP(K3)))</f>
-        <v>1.7594723053576653E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" s="22" customFormat="1"/>
-    <row r="50" spans="2:14" s="22" customFormat="1"/>
-    <row r="51" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
-    <row r="52" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1">
-      <c r="G52"/>
-      <c r="H52" s="51">
-        <f>F4</f>
-        <v>1.35</v>
-      </c>
-      <c r="I52" s="52">
-        <f t="shared" ref="I52:J52" si="9">G4</f>
-        <v>1.27</v>
-      </c>
-      <c r="J52" s="53">
-        <f t="shared" si="9"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" s="22" customFormat="1" ht="15.75">
-      <c r="E53" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="50"/>
-      <c r="G53" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H53" s="54">
-        <f>H52</f>
-        <v>1.35</v>
-      </c>
-      <c r="I53" s="21">
-        <f t="shared" ref="I53:I54" si="10">I52</f>
-        <v>1.27</v>
-      </c>
-      <c r="J53" s="55">
-        <f t="shared" ref="J53:J54" si="11">J52</f>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="G54"/>
-      <c r="H54" s="56">
-        <f>H53</f>
-        <v>1.35</v>
-      </c>
-      <c r="I54" s="57">
-        <f t="shared" si="10"/>
-        <v>1.27</v>
-      </c>
-      <c r="J54" s="58">
-        <f t="shared" si="11"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1"/>
-    <row r="56" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1"/>
-    <row r="57" spans="2:14" s="22" customFormat="1" ht="15.75">
-      <c r="E57" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F57" s="50"/>
-      <c r="G57" s="47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1"/>
-    <row r="59" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1"/>
-    <row r="60" spans="2:14" s="22" customFormat="1" ht="12" customHeight="1"/>
-    <row r="61" spans="2:14" s="22" customFormat="1"/>
-    <row r="62" spans="2:14" s="22" customFormat="1"/>
-    <row r="63" spans="2:14" s="22" customFormat="1">
-      <c r="N63" s="42">
-        <f>EXP(N3)*(EXP(L3)+EXP(M3))/(EXP(L3)+EXP(M3)+EXP(N3))^2</f>
-        <v>0.24973763855303174</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" s="2" customFormat="1">
-      <c r="B64" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="2">
-        <f>1/(1+EXP(I3))*(1-1/(1+EXP(I3)))</f>
-        <v>5.7427099367579122E-2</v>
-      </c>
-      <c r="J64" s="2">
-        <f>1/(1+EXP(J3))*(1-1/(1+EXP(J3)))</f>
-        <v>5.5981215831597007E-2</v>
-      </c>
-      <c r="K64" s="2">
-        <f>1/(1+EXP(K3))*(1-1/(1+EXP(K3)))</f>
-        <v>1.7594723053576653E-2</v>
-      </c>
-      <c r="L64" s="2">
-        <f>(EXP(L3)*(EXP(M3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
-        <v>0.15906572440211431</v>
-      </c>
-      <c r="M64" s="2">
-        <f>(EXP(M3)*(EXP(L3)+EXP(N3)))/(EXP($L$3)+EXP($M$3)+EXP($N$3))^2</f>
-        <v>0.20392775168086905</v>
-      </c>
-      <c r="N64" s="24">
-        <v>0.36849999999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" s="35" customFormat="1">
-      <c r="A65" s="37"/>
-      <c r="B65" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="L65" s="35">
-        <f>SUM(L66:L68)</f>
-        <v>-3.7065529644704216</v>
-      </c>
-      <c r="M65" s="35">
-        <f>SUM(M66:M68)</f>
-        <v>-1.4755293951978394</v>
-      </c>
-      <c r="N65" s="35">
-        <f>SUM(N66:N68)</f>
-        <v>-1.6889906479667314</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" s="3" customFormat="1">
-      <c r="A66" s="36"/>
-      <c r="B66" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I66" s="3">
-        <f>L66*L64*I69</f>
-        <v>-0.55352134557837929</v>
-      </c>
-      <c r="L66" s="3">
-        <f>(-1)*(C11*(1/L4)+(1-C11)*(1/(1-L4)))</f>
-        <v>-3.7065529644704216</v>
-      </c>
-      <c r="M66" s="3">
-        <v>0</v>
-      </c>
-      <c r="N66" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" s="3" customFormat="1">
-      <c r="A67" s="36"/>
-      <c r="B67" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L67" s="3">
-        <v>0</v>
-      </c>
-      <c r="M67" s="3">
-        <f>(-1)*(D11*(1/M4)+(1-D11)*(1/(1-M4)))</f>
-        <v>-1.4755293951978394</v>
-      </c>
-      <c r="N67" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A68" s="36"/>
-      <c r="B68" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0</v>
-      </c>
-      <c r="M68" s="3">
-        <v>0</v>
-      </c>
-      <c r="N68" s="3">
-        <f>(-1)*(E11*(1/N4)+(1-E11)*(1/(1-N4)))</f>
-        <v>-1.6889906479667314</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" s="2" customFormat="1">
-      <c r="B69" s="38" t="s">
+    <row r="139" spans="1:14" s="2" customFormat="1">
+      <c r="B139" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="8">
+      <c r="F139" s="8">
         <f>F$4</f>
         <v>1.35</v>
       </c>
-      <c r="G69" s="9">
-        <f>F69</f>
+      <c r="G139" s="9">
+        <f t="shared" ref="G139:H141" si="28">F139</f>
         <v>1.35</v>
       </c>
-      <c r="H69" s="10">
-        <f>G69</f>
+      <c r="H139" s="10">
+        <f t="shared" si="28"/>
         <v>1.35</v>
       </c>
-      <c r="I69" s="8">
+      <c r="I139" s="8">
         <f>I$4</f>
         <v>0.9388312894865416</v>
       </c>
-      <c r="J69" s="9">
-        <f>I69</f>
+      <c r="J139" s="9">
+        <f t="shared" ref="J139:K141" si="29">I139</f>
         <v>0.9388312894865416</v>
       </c>
-      <c r="K69" s="10">
-        <f>J69</f>
+      <c r="K139" s="10">
+        <f t="shared" si="29"/>
         <v>0.9388312894865416</v>
       </c>
     </row>
-    <row r="70" spans="1:14" s="2" customFormat="1">
-      <c r="B70" s="38"/>
-      <c r="F70" s="15">
+    <row r="140" spans="1:14" s="2" customFormat="1">
+      <c r="B140" s="59"/>
+      <c r="F140" s="15">
         <f>G$4</f>
         <v>1.27</v>
       </c>
-      <c r="G70" s="16">
-        <f t="shared" ref="G70:H70" si="12">F70</f>
+      <c r="G140" s="16">
+        <f t="shared" si="28"/>
         <v>1.27</v>
       </c>
-      <c r="H70" s="17">
-        <f t="shared" si="12"/>
+      <c r="H140" s="17">
+        <f t="shared" si="28"/>
         <v>1.27</v>
       </c>
-      <c r="I70" s="15">
+      <c r="I140" s="15">
         <f>J$4</f>
         <v>0.94047563402349843</v>
       </c>
-      <c r="J70" s="16">
-        <f t="shared" ref="J70:K70" si="13">I70</f>
+      <c r="J140" s="16">
+        <f t="shared" si="29"/>
         <v>0.94047563402349843</v>
       </c>
-      <c r="K70" s="17">
-        <f t="shared" si="13"/>
+      <c r="K140" s="17">
+        <f t="shared" si="29"/>
         <v>0.94047563402349843</v>
       </c>
     </row>
-    <row r="71" spans="1:14" s="2" customFormat="1" ht="13.5" thickBot="1">
-      <c r="B71" s="38"/>
-      <c r="F71" s="18">
+    <row r="141" spans="1:14" s="2" customFormat="1" ht="13.5" thickBot="1">
+      <c r="B141" s="59"/>
+      <c r="F141" s="18">
         <f>H$4</f>
         <v>1.8</v>
       </c>
-      <c r="G71" s="19">
-        <f t="shared" ref="G71:H71" si="14">F71</f>
+      <c r="G141" s="19">
+        <f t="shared" si="28"/>
         <v>1.8</v>
       </c>
-      <c r="H71" s="20">
-        <f t="shared" si="14"/>
+      <c r="H141" s="20">
+        <f t="shared" si="28"/>
         <v>1.8</v>
       </c>
-      <c r="I71" s="18">
+      <c r="I141" s="18">
         <f>K$4</f>
         <v>0.9820843048123673</v>
       </c>
-      <c r="J71" s="19">
-        <f t="shared" ref="J71:K71" si="15">I71</f>
+      <c r="J141" s="19">
+        <f t="shared" si="29"/>
         <v>0.9820843048123673</v>
       </c>
-      <c r="K71" s="20">
-        <f t="shared" si="15"/>
+      <c r="K141" s="20">
+        <f t="shared" si="29"/>
         <v>0.9820843048123673</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="25" customFormat="1"/>
-    <row r="73" spans="1:14" s="25" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="74" spans="1:14" s="25" customFormat="1">
-      <c r="B74" s="38" t="s">
+    <row r="142" spans="1:14" s="25" customFormat="1"/>
+    <row r="143" spans="1:14" s="25" customFormat="1" ht="13.5" thickBot="1"/>
+    <row r="144" spans="1:14" s="25" customFormat="1">
+      <c r="B144" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="I74" s="26">
-        <f>I69*L$64*L$66</f>
+      <c r="I144" s="26">
+        <f>I139*L$134*L$136</f>
         <v>-0.55352134557837929</v>
       </c>
-      <c r="J74" s="27">
-        <f>J69*M$64*M$67</f>
+      <c r="J144" s="27">
+        <f>J139*M$134*M$137</f>
         <v>-0.28249564195516064</v>
       </c>
-      <c r="K74" s="28">
-        <f>K69*N$64*N$68</f>
+      <c r="K144" s="28">
+        <f>K139*N$134*N$138</f>
         <v>-0.58432207324374486</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="25" customFormat="1">
-      <c r="B75" s="38"/>
-      <c r="I75" s="29">
-        <f>I70*L$64*L$66</f>
+    <row r="145" spans="2:11" s="25" customFormat="1">
+      <c r="B145" s="59"/>
+      <c r="I145" s="29">
+        <f>I140*L$134*L$136</f>
         <v>-0.55449082732753208</v>
       </c>
-      <c r="J75" s="30">
-        <f>J70*M$64*M$67</f>
+      <c r="J145" s="30">
+        <f>J140*M$134*M$137</f>
         <v>-0.28299042751542586</v>
       </c>
-      <c r="K75" s="31">
-        <f>K70*N$64*N$68</f>
+      <c r="K145" s="31">
+        <f>K140*N$134*N$138</f>
         <v>-0.58534550186156087</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="25" customFormat="1" ht="13.5" thickBot="1">
-      <c r="B76" s="38"/>
-      <c r="I76" s="32">
-        <f>I71*L$64*L$66</f>
+    <row r="146" spans="2:11" s="25" customFormat="1" ht="13.5" thickBot="1">
+      <c r="B146" s="59"/>
+      <c r="I146" s="32">
+        <f>I141*L$134*L$136</f>
         <v>-0.57902269764406011</v>
       </c>
-      <c r="J76" s="33">
-        <f>J71*M$64*M$67</f>
+      <c r="J146" s="33">
+        <f>J141*M$134*M$137</f>
         <v>-0.29551053447929898</v>
       </c>
-      <c r="K76" s="34">
-        <f>K71*N$64*N$68</f>
+      <c r="K146" s="34">
+        <f>K141*N$134*N$138</f>
         <v>-0.61124244953739448</v>
       </c>
     </row>
-    <row r="77" spans="1:14" s="25" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="78" spans="1:14" s="25" customFormat="1">
-      <c r="B78" s="38" t="s">
+    <row r="147" spans="2:11" s="25" customFormat="1" ht="13.5" thickBot="1"/>
+    <row r="148" spans="2:11" s="25" customFormat="1">
+      <c r="B148" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="I78" s="26">
-        <f>I5-$S$3*I74</f>
+      <c r="I148" s="26">
+        <f>I5-$S$3*I144</f>
         <v>0.1055352134557838</v>
       </c>
-      <c r="J78" s="27">
-        <f>J5-$S$3*J74</f>
+      <c r="J148" s="27">
+        <f>J5-$S$3*J144</f>
         <v>0.40282495641955163</v>
       </c>
-      <c r="K78" s="28">
-        <f>K5-$S$3*K74</f>
+      <c r="K148" s="28">
+        <f>K5-$S$3*K144</f>
         <v>0.80584322073243753</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="25" customFormat="1">
-      <c r="B79" s="38"/>
-      <c r="I79" s="29">
-        <f>I6-$S$3*I75</f>
+    <row r="149" spans="2:11" s="25" customFormat="1">
+      <c r="B149" s="59"/>
+      <c r="I149" s="29">
+        <f>I6-$S$3*I145</f>
         <v>0.3055449082732753</v>
       </c>
-      <c r="J79" s="30">
-        <f>J6-$S$3*J75</f>
+      <c r="J149" s="30">
+        <f>J6-$S$3*J145</f>
         <v>0.70282990427515424</v>
       </c>
-      <c r="K79" s="31">
-        <f>K6-$S$3*K75</f>
+      <c r="K149" s="31">
+        <f>K6-$S$3*K145</f>
         <v>0.20585345501861563</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="25" customFormat="1" ht="13.5" thickBot="1">
-      <c r="B80" s="38"/>
-      <c r="I80" s="32">
-        <f>I7-$S$3*I76</f>
+    <row r="150" spans="2:11" s="25" customFormat="1" ht="13.5" thickBot="1">
+      <c r="B150" s="59"/>
+      <c r="I150" s="32">
+        <f>I7-$S$3*I146</f>
         <v>0.5057902269764406</v>
       </c>
-      <c r="J80" s="33">
-        <f>J7-$S$3*J76</f>
+      <c r="J150" s="33">
+        <f>J7-$S$3*J146</f>
         <v>0.202955105344793</v>
       </c>
-      <c r="K80" s="34">
-        <f>K7-$S$3*K76</f>
+      <c r="K150" s="34">
+        <f>K7-$S$3*K146</f>
         <v>0.90611242449537399</v>
       </c>
     </row>
-    <row r="81" spans="2:2" s="25" customFormat="1"/>
-    <row r="82" spans="2:2" s="25" customFormat="1"/>
-    <row r="83" spans="2:2" s="25" customFormat="1"/>
-    <row r="84" spans="2:2" s="25" customFormat="1">
-      <c r="B84" s="3" t="s">
+    <row r="151" spans="2:11" s="25" customFormat="1"/>
+    <row r="152" spans="2:11" s="25" customFormat="1"/>
+    <row r="153" spans="2:11" s="25" customFormat="1"/>
+    <row r="154" spans="2:11" s="25" customFormat="1">
+      <c r="B154" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="2:2" s="25" customFormat="1"/>
-    <row r="86" spans="2:2" s="25" customFormat="1"/>
-    <row r="87" spans="2:2" s="25" customFormat="1"/>
-    <row r="88" spans="2:2" s="25" customFormat="1"/>
-    <row r="89" spans="2:2" s="25" customFormat="1"/>
-    <row r="90" spans="2:2" s="25" customFormat="1"/>
-    <row r="91" spans="2:2" s="25" customFormat="1"/>
-    <row r="92" spans="2:2" s="25" customFormat="1"/>
-    <row r="93" spans="2:2" s="25" customFormat="1"/>
-    <row r="94" spans="2:2" s="25" customFormat="1"/>
-    <row r="95" spans="2:2" s="25" customFormat="1"/>
-    <row r="96" spans="2:2" s="25" customFormat="1"/>
-    <row r="97" s="25" customFormat="1"/>
-    <row r="98" s="25" customFormat="1"/>
+    <row r="155" spans="2:11" s="25" customFormat="1"/>
+    <row r="156" spans="2:11" s="25" customFormat="1"/>
+    <row r="157" spans="2:11" s="25" customFormat="1"/>
+    <row r="158" spans="2:11" s="25" customFormat="1"/>
+    <row r="159" spans="2:11" s="25" customFormat="1"/>
+    <row r="160" spans="2:11" s="25" customFormat="1"/>
+    <row r="161" s="25" customFormat="1"/>
+    <row r="162" s="25" customFormat="1"/>
+    <row r="163" s="25" customFormat="1"/>
+    <row r="164" s="25" customFormat="1"/>
+    <row r="165" s="25" customFormat="1"/>
+    <row r="166" s="25" customFormat="1"/>
+    <row r="167" s="25" customFormat="1"/>
+    <row r="168" s="25" customFormat="1"/>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="37">
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="U75:V75"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="K99:L99"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E127:F127"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L94:M94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2353,22 +3928,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2378,9 +3941,15 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Forward and ErrorEvaluatorEnum ready
</commit_message>
<xml_diff>
--- a/NeuralNetwork/ExternalFiles/Nn.xlsx
+++ b/NeuralNetwork/ExternalFiles/Nn.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
   <si>
     <t>Input</t>
   </si>
@@ -945,6 +945,9 @@
       </rPr>
       <t xml:space="preserve"> =</t>
     </r>
+  </si>
+  <si>
+    <t>??? - de ce exista doar crossentropy prim si nu exista si neprim?</t>
   </si>
 </sst>
 </file>
@@ -1581,6 +1584,39 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1589,39 +1625,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1661,7 +1664,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="https://cdn-images-1.medium.com/max/1600/1*fdDRKoUj5ck2k4Aa2BSaAA.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{635E3D66-EA89-49A8-8B2C-2AFE732D2B64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{635E3D66-EA89-49A8-8B2C-2AFE732D2B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1722,7 +1725,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="https://cdn-images-1.medium.com/max/1600/1*XWyzdij1A-RpkqPNbm9Lrw.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17ECD454-2D91-450B-B800-19D2DCFB63D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17ECD454-2D91-450B-B800-19D2DCFB63D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1768,22 +1771,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>113264</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>589514</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4" descr="https://cdn-images-1.medium.com/max/1600/1*NWb_tAHWvBwJc0hNm0LiUQ.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EA436DA-C610-48C6-BC7B-27EB73C67899}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0EA436DA-C610-48C6-BC7B-27EB73C67899}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1806,7 +1809,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1457325" y="10096500"/>
+          <a:off x="714375" y="7019925"/>
           <a:ext cx="4085189" cy="2228849"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2128,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2142,43 +2145,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" thickBot="1">
-      <c r="F1" s="130" t="s">
+      <c r="F1" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130" t="s">
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130" t="s">
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" thickBot="1">
-      <c r="C2" s="128" t="s">
+      <c r="C2" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="129" t="s">
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129" t="s">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129" t="s">
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
       <c r="S2" s="120" t="s">
         <v>21</v>
       </c>
@@ -2258,15 +2261,15 @@
         <f>E3</f>
         <v>0.7</v>
       </c>
-      <c r="F4" s="133">
+      <c r="F4" s="122">
         <f>MAX(0,F3)</f>
         <v>1.35</v>
       </c>
-      <c r="G4" s="134">
+      <c r="G4" s="123">
         <f>MAX(0,G3)</f>
         <v>1.27</v>
       </c>
-      <c r="H4" s="135">
+      <c r="H4" s="124">
         <f>MAX(0,H3)</f>
         <v>1.8</v>
       </c>
@@ -2296,7 +2299,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="135" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2334,7 +2337,7 @@
       <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:26" s="2" customFormat="1">
-      <c r="A6" s="124"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2370,7 +2373,7 @@
       <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:26" s="2" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A7" s="124"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2445,21 +2448,21 @@
     </row>
     <row r="9" spans="1:26" s="24" customFormat="1">
       <c r="A9" s="96"/>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131" t="s">
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="131"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="131" t="s">
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="128"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
@@ -2531,9 +2534,18 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="G13" s="21">
+        <f>(-1)*(C12*(1/L4)+(1-C12)*(1/(1-L4)))</f>
+        <v>-5.039131521137528</v>
+      </c>
+      <c r="H13" s="21">
+        <f>(-1)*(D12*(1/M4)+(1-D12)*(1/(1-M4)))</f>
+        <v>-1.3992971926232187</v>
+      </c>
+      <c r="I13" s="21">
+        <f>(-1)*(E12*(1/N4)+(1-E12)*(1/(1-N4)))</f>
+        <v>-2.066959463271492</v>
+      </c>
     </row>
     <row r="14" spans="1:26" s="22" customFormat="1" ht="16.5" thickBot="1">
       <c r="I14" s="33" t="s">
@@ -2557,7 +2569,9 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="T14" s="32"/>
+      <c r="T14" s="32" t="s">
+        <v>76</v>
+      </c>
       <c r="U14" s="32"/>
       <c r="V14" s="32"/>
       <c r="X14" s="32"/>
@@ -2582,7 +2596,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" s="22" customFormat="1" ht="15.75">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="133" t="s">
         <v>33</v>
       </c>
       <c r="D17"/>
@@ -2611,7 +2625,7 @@
       </c>
     </row>
     <row r="18" spans="1:27" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A18" s="123"/>
+      <c r="A18" s="134"/>
       <c r="T18" s="79">
         <v>0</v>
       </c>
@@ -2660,13 +2674,13 @@
       </c>
     </row>
     <row r="23" spans="1:27" s="22" customFormat="1" ht="15.75">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="133" t="s">
         <v>34</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="132" t="s">
+      <c r="H23" s="129" t="s">
         <v>40</v>
       </c>
       <c r="I23" s="125"/>
@@ -2707,7 +2721,7 @@
       </c>
     </row>
     <row r="24" spans="1:27" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A24" s="123"/>
+      <c r="A24" s="134"/>
       <c r="K24" s="71">
         <v>0</v>
       </c>
@@ -3042,11 +3056,11 @@
         <v>0.8</v>
       </c>
       <c r="T39" s="74">
-        <f t="shared" ref="T39:V41" si="13">$T22*K$39+$U22*K$40+$V22*K$41</f>
+        <f>$T22*K$39+$U22*K$40+$V22*K$41</f>
         <v>-8.0155310576726924E-2</v>
       </c>
       <c r="U39" s="75">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="T39:V41" si="13">$T22*L$39+$U22*L$40+$V22*L$41</f>
         <v>-0.32062124230690769</v>
       </c>
       <c r="V39" s="76">
@@ -4195,30 +4209,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="Q79:R79"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="Q69:R69"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A5:A7"/>
@@ -4235,6 +4225,30 @@
     <mergeCell ref="Q23:R23"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="Q56:R56"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="Q79:R79"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="Q69:R69"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="Q74:R74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>